<commit_message>
Novas instrucoes do Prof. Samuel
</commit_message>
<xml_diff>
--- a/metadados/mapa_das _bases.xlsx
+++ b/metadados/mapa_das _bases.xlsx
@@ -13,9 +13,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="319">
-  <si>
-    <t>fia_marketing_push</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="317">
+  <si>
+    <t>fia_marketing_push_full</t>
   </si>
   <si>
     <t>fia_customer_segmentation</t>
@@ -209,63 +209,52 @@
 quando houver esse dado</t>
   </si>
   <si>
+    <t>External_user_id</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>qtt_valid_orders</t>
+  </si>
+  <si>
+    <t>Contagem de pedidos validos na vida ( last_status != 'CANCELLED' ).</t>
+  </si>
+  <si>
+    <t>last_status_date_local</t>
+  </si>
+  <si>
+    <t>data do último status do pedido no timezone do pedido</t>
+  </si>
+  <si>
+    <t>frn_id</t>
+  </si>
+  <si>
+    <t>short id do restaurante</t>
+  </si>
+  <si>
+    <t>session_started_at_amsp</t>
+  </si>
+  <si>
+    <t>Data e hora de início da sessão no fuso América/São Paul</t>
+  </si>
+  <si>
     <t>event_time_utc3</t>
   </si>
   <si>
     <t>timestamp utc3 do evento</t>
   </si>
   <si>
-    <t>qtt_valid_orders</t>
-  </si>
-  <si>
-    <t>Contagem de pedidos validos na vida ( last_status != 'CANCELLED' ).</t>
-  </si>
-  <si>
-    <t>last_status</t>
-  </si>
-  <si>
-    <t>último status do pedido. Status possíveis:
-(status sem *** são status temporarios do pedido)
-CONCLUDED*** (pedidos ok)
-CONFIRMED
-ERROR
-DISPATCHED
-REGISTERED
-GOING_TO_DESTINATION
-None
-ARRIVED_AT_DESTINATION
-ARRIVED
-ARRIVED_AT_ORIGIN
-CANCELLED *** (pedidos que deram rpoblema)
-REJECTED
-PLACED
-GOING_TO_ORIGIN
-PENDING
-UNDEFINED</t>
-  </si>
-  <si>
-    <t>frn_id</t>
-  </si>
-  <si>
-    <t>short id do restaurante</t>
-  </si>
-  <si>
-    <t>session_started_at_amsp</t>
-  </si>
-  <si>
-    <t>Data e hora de início da sessão no fuso América/São Paul</t>
-  </si>
-  <si>
     <t>last_valid_order_date</t>
   </si>
   <si>
     <t>Data do último pedido validos.</t>
   </si>
   <si>
-    <t>last_status_date_local</t>
-  </si>
-  <si>
-    <t>data do último status do pedido no timezone do pedido</t>
+    <t>order_total</t>
+  </si>
+  <si>
+    <t>valor total do pedido (order_items_total + delivery_fee)</t>
   </si>
   <si>
     <t>order_date_local</t>
@@ -280,58 +269,61 @@
     <t>Data e hora de término da sessão no fuso América/São Paulo</t>
   </si>
   <si>
+    <t>qtt_invalid_orders</t>
+  </si>
+  <si>
+    <t>Contagem de pedidos inválidos na vida ( last_status = 'CONCLUDED').</t>
+  </si>
+  <si>
+    <t>credit</t>
+  </si>
+  <si>
+    <t>valor total de desconto no pedido</t>
+  </si>
+  <si>
+    <t>general_net_profit</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Receitas menos os custos (lucro)</t>
+  </si>
+  <si>
+    <t>session_started_at_utc0</t>
+  </si>
+  <si>
+    <t>Data e hora de início da sessão dentro do UTC0</t>
+  </si>
+  <si>
     <t>campaign_id</t>
   </si>
   <si>
     <t>uuid de identificação da campanha</t>
   </si>
   <si>
-    <t>qtt_invalid_orders</t>
-  </si>
-  <si>
-    <t>Contagem de pedidos inválidos na vida ( last_status = 'CONCLUDED').</t>
-  </si>
-  <si>
-    <t>order_total</t>
-  </si>
-  <si>
-    <t>valor total do pedido (order_items_total + delivery_fee)</t>
-  </si>
-  <si>
-    <t>session_started_at_utc0</t>
-  </si>
-  <si>
-    <t>Data e hora de início da sessão dentro do UTC0</t>
+    <t>last_invalid_order_date</t>
+  </si>
+  <si>
+    <t>Data do último pedido inválido.</t>
+  </si>
+  <si>
+    <t>paid_amount</t>
+  </si>
+  <si>
+    <t>valor pago no pedido pelo usuário</t>
+  </si>
+  <si>
+    <t>session_ended_at_utc0</t>
+  </si>
+  <si>
+    <t>Data e hora de término da sessão dentro do UTC0</t>
   </si>
   <si>
     <t>campaign_name</t>
   </si>
   <si>
     <t>nome da campanha (com base em alguns filtros e uma segmentação rola um envio)</t>
-  </si>
-  <si>
-    <t>last_invalid_order_date</t>
-  </si>
-  <si>
-    <t>Data do último pedido inválido.</t>
-  </si>
-  <si>
-    <t>credit</t>
-  </si>
-  <si>
-    <t>valor total de desconto no pedido</t>
-  </si>
-  <si>
-    <t>session_ended_at_utc0</t>
-  </si>
-  <si>
-    <t>Data e hora de término da sessão dentro do UTC0</t>
-  </si>
-  <si>
-    <t>message_variation_channel</t>
-  </si>
-  <si>
-    <t>canal de envio da variante</t>
   </si>
   <si>
     <t>marlin_tag</t>
@@ -344,10 +336,10 @@
 </t>
   </si>
   <si>
-    <t>paid_amount</t>
-  </si>
-  <si>
-    <t>valor pago no pedido pelo usuário</t>
+    <t>delivery_type</t>
+  </si>
+  <si>
+    <t>tipo de entrega (delivery ou takeout)</t>
   </si>
   <si>
     <t>session_duration_seconds</t>
@@ -361,28 +353,55 @@
 convertido no formato utc</t>
   </si>
   <si>
+    <t>message_variation_channel</t>
+  </si>
+  <si>
+    <t>canal de envio da variante</t>
+  </si>
+  <si>
+    <t>recency_months</t>
+  </si>
+  <si>
+    <t>Meses desde o último pedido.</t>
+  </si>
+  <si>
+    <t>scheduled</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>booleano que indica que houve agendamento do pedido</t>
+  </si>
+  <si>
+    <t>device_model</t>
+  </si>
+  <si>
+    <t>Modelo do dispositivo, definido pelo campo entity_device_model</t>
+  </si>
+  <si>
     <t>canvas_name</t>
   </si>
   <si>
     <t>nome do canvas (encadeamente de varias campanhas e determinar um filtro/evento pra cada uma acontecer)</t>
   </si>
   <si>
-    <t>recency_months</t>
-  </si>
-  <si>
-    <t>Meses desde o último pedido.</t>
-  </si>
-  <si>
-    <t>delivery_type</t>
-  </si>
-  <si>
-    <t>tipo de entrega (delivery ou takeout)</t>
-  </si>
-  <si>
-    <t>device_model</t>
-  </si>
-  <si>
-    <t>Modelo do dispositivo, definido pelo campo entity_device_model</t>
+    <t>last_nps</t>
+  </si>
+  <si>
+    <t>Última avaliação de NPS no app.</t>
+  </si>
+  <si>
+    <t>scheduled_creation_date_local</t>
+  </si>
+  <si>
+    <t>data de criação do agendamento do pedido (horário local)</t>
+  </si>
+  <si>
+    <t>device_manufacturer</t>
+  </si>
+  <si>
+    <t>Fabricante do dispositivo, definido pelo campo entity_manufacturer</t>
   </si>
   <si>
     <t>canvas_step_id</t>
@@ -391,25 +410,22 @@
     <t>step do canvas que enviou o push</t>
   </si>
   <si>
-    <t>last_nps</t>
-  </si>
-  <si>
-    <t>Última avaliação de NPS no app.</t>
-  </si>
-  <si>
-    <t>scheduled</t>
-  </si>
-  <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t>booleano que indica que houve agendamento do pedido</t>
-  </si>
-  <si>
-    <t>device_manufacturer</t>
-  </si>
-  <si>
-    <t>Fabricante do dispositivo, definido pelo campo entity_manufacturer</t>
+    <t>registration_date</t>
+  </si>
+  <si>
+    <t>Data de registro do usuário.</t>
+  </si>
+  <si>
+    <t>device_app_version</t>
+  </si>
+  <si>
+    <t>versão do app utilizado no pedido</t>
+  </si>
+  <si>
+    <t>sum_event_open</t>
+  </si>
+  <si>
+    <t>Quantidade de eventos de abertura do Aplicativo durante a sessão.</t>
   </si>
   <si>
     <t>canvas_is_first_step</t>
@@ -421,22 +437,22 @@
     <t>indentificação se o step é o primeiro da variante</t>
   </si>
   <si>
-    <t>registration_date</t>
-  </si>
-  <si>
-    <t>Data de registro do usuário.</t>
-  </si>
-  <si>
-    <t>scheduled_creation_date_local</t>
-  </si>
-  <si>
-    <t>data de criação do agendamento do pedido (horário local)</t>
-  </si>
-  <si>
-    <t>sum_event_open</t>
-  </si>
-  <si>
-    <t>Quantidade de eventos de abertura do Aplicativo durante a sessão.</t>
+    <t>customer_lifetime_days</t>
+  </si>
+  <si>
+    <t>Dias desde o primeiro pedido do usuário.</t>
+  </si>
+  <si>
+    <t>device_type</t>
+  </si>
+  <si>
+    <t>tipo de ambiente utilizado no pedido (Mobile/Site)</t>
+  </si>
+  <si>
+    <t>sum_view_restaurant_screen</t>
+  </si>
+  <si>
+    <t>Quantidade de eventos de visualizações da tela do restaurante</t>
   </si>
   <si>
     <t>canvas_first_step_name</t>
@@ -445,22 +461,22 @@
     <t>nome do primeiro step do canvas</t>
   </si>
   <si>
-    <t>customer_lifetime_days</t>
-  </si>
-  <si>
-    <t>Dias desde o primeiro pedido do usuário.</t>
-  </si>
-  <si>
-    <t>device_app_version</t>
-  </si>
-  <si>
-    <t>versão do app utilizado no pedido</t>
-  </si>
-  <si>
-    <t>sum_view_restaurant_screen</t>
-  </si>
-  <si>
-    <t>Quantidade de eventos de visualizações da tela do restaurante</t>
+    <t>customer_lifetime_months</t>
+  </si>
+  <si>
+    <t>Meses desde o primeiro pedido do usuário.</t>
+  </si>
+  <si>
+    <t>device_platform</t>
+  </si>
+  <si>
+    <t>plataforma do device (iOS/Android/Desktop)</t>
+  </si>
+  <si>
+    <t>sum_view_dish_screen</t>
+  </si>
+  <si>
+    <t>Quantidade de eventos de visualizações da tela de pratos</t>
   </si>
   <si>
     <t>canvas_step_name</t>
@@ -469,22 +485,25 @@
     <t>nome da variante</t>
   </si>
   <si>
-    <t>customer_lifetime_months</t>
-  </si>
-  <si>
-    <t>Meses desde o primeiro pedido do usuário.</t>
-  </si>
-  <si>
-    <t>device_type</t>
-  </si>
-  <si>
-    <t>tipo de ambiente utilizado no pedido (Mobile/Site)</t>
-  </si>
-  <si>
-    <t>sum_view_dish_screen</t>
-  </si>
-  <si>
-    <t>Quantidade de eventos de visualizações da tela de pratos</t>
+    <t>top_3_merchants_code</t>
+  </si>
+  <si>
+    <t>array</t>
+  </si>
+  <si>
+    <t>merchant_id dos top 3 merchants em que o usuário mais pediu.</t>
+  </si>
+  <si>
+    <t>payment_method</t>
+  </si>
+  <si>
+    <t>método de pagamento (Online/Offline)</t>
+  </si>
+  <si>
+    <t>sum_click_add_item</t>
+  </si>
+  <si>
+    <t>Quantidade de eventos de click do botão Add itens</t>
   </si>
   <si>
     <t>canvas_real_step_name</t>
@@ -493,25 +512,22 @@
     <t>nome do step do canvas</t>
   </si>
   <si>
-    <t>top_3_merchants_code</t>
-  </si>
-  <si>
-    <t>array</t>
-  </si>
-  <si>
-    <t>merchant_id dos top 3 merchants em que o usuário mais pediu.</t>
-  </si>
-  <si>
-    <t>device_platform</t>
-  </si>
-  <si>
-    <t>plataforma do device (iOS/Android/Desktop)</t>
-  </si>
-  <si>
-    <t>sum_click_add_item</t>
-  </si>
-  <si>
-    <t>Quantidade de eventos de click do botão Add itens</t>
+    <t>was_mub_last_month</t>
+  </si>
+  <si>
+    <t>booleano se o usuário foi mub no mês passado.</t>
+  </si>
+  <si>
+    <t>customer_state_label</t>
+  </si>
+  <si>
+    <t>estado de entrega do usuário</t>
+  </si>
+  <si>
+    <t>sum_view_checkout</t>
+  </si>
+  <si>
+    <t>Quantidade de eventos de visualizações do checkout</t>
   </si>
   <si>
     <t>canvas_step_index</t>
@@ -520,22 +536,22 @@
     <t>indice do step (posição do step em relação a variante)</t>
   </si>
   <si>
-    <t>was_mub_last_month</t>
-  </si>
-  <si>
-    <t>booleano se o usuário foi mub no mês passado.</t>
-  </si>
-  <si>
-    <t>payment_method</t>
-  </si>
-  <si>
-    <t>método de pagamento (Online/Offline)</t>
-  </si>
-  <si>
-    <t>sum_view_checkout</t>
-  </si>
-  <si>
-    <t>Quantidade de eventos de visualizações do checkout</t>
+    <t>buyer_last_91d</t>
+  </si>
+  <si>
+    <t>booleano se o usuário fez pelo menos uma compra nos últimos 91 dias.</t>
+  </si>
+  <si>
+    <t>customer_city</t>
+  </si>
+  <si>
+    <t>cidade de entrega do usuário</t>
+  </si>
+  <si>
+    <t>sum_callback_purchase</t>
+  </si>
+  <si>
+    <t>Quantidade de eventos de Callback de pedidos</t>
   </si>
   <si>
     <t>canvas_tags</t>
@@ -544,22 +560,22 @@
     <t>array com as tags do canvas (tags são utilizadas para facilitar a busca por canvas dentro do Braze)</t>
   </si>
   <si>
-    <t>buyer_last_91d</t>
-  </si>
-  <si>
-    <t>booleano se o usuário fez pelo menos uma compra nos últimos 91 dias.</t>
-  </si>
-  <si>
-    <t>customer_state_label</t>
-  </si>
-  <si>
-    <t>estado de entrega do usuário</t>
-  </si>
-  <si>
-    <t>sum_callback_purchase</t>
-  </si>
-  <si>
-    <t>Quantidade de eventos de Callback de pedidos</t>
+    <t>top_city</t>
+  </si>
+  <si>
+    <t>Cidade em que o usuário realizou mais pedidos.</t>
+  </si>
+  <si>
+    <t>customer_district</t>
+  </si>
+  <si>
+    <t>bairro de entrega do usuário</t>
+  </si>
+  <si>
+    <t>order_session_quantity</t>
+  </si>
+  <si>
+    <t>Quantidade de pedidos com sucesso por sessão</t>
   </si>
   <si>
     <t>send_id</t>
@@ -568,22 +584,22 @@
     <t>id do envio</t>
   </si>
   <si>
-    <t>top_city</t>
-  </si>
-  <si>
-    <t>Cidade em que o usuário realizou mais pedidos.</t>
-  </si>
-  <si>
-    <t>customer_city</t>
-  </si>
-  <si>
-    <t>cidade de entrega do usuário</t>
-  </si>
-  <si>
-    <t>order_session_quantity</t>
-  </si>
-  <si>
-    <t>Quantidade de pedidos com sucesso por sessão</t>
+    <t>top_district</t>
+  </si>
+  <si>
+    <t>Bairro em que o usuário realizou mais pedidos.</t>
+  </si>
+  <si>
+    <t>customer_centroid_id</t>
+  </si>
+  <si>
+    <t>representação do centroide do usuário (concatenado do lat/long do usuário, com duas casas decimais)</t>
+  </si>
+  <si>
+    <t>first_order_origin_feature</t>
+  </si>
+  <si>
+    <t>De qual feature veio a compra. Se foi de uma lista, de uma busca, ou outro.</t>
   </si>
   <si>
     <t>event_date</t>
@@ -592,37 +608,16 @@
     <t>data do envio</t>
   </si>
   <si>
-    <t>top_district</t>
-  </si>
-  <si>
-    <t>Bairro em que o usuário realizou mais pedidos.</t>
-  </si>
-  <si>
-    <t>customer_district</t>
-  </si>
-  <si>
-    <t>bairro de entrega do usuário</t>
-  </si>
-  <si>
-    <t>first_order_origin_feature</t>
-  </si>
-  <si>
-    <t>De qual feature veio a compra. Se foi de uma lista, de uma busca, ou outro.</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>top_centroid_id</t>
   </si>
   <si>
     <t>Top centroid_id em que o usuário realizou mais pedidos.</t>
   </si>
   <si>
-    <t>customer_longitude</t>
-  </si>
-  <si>
-    <t>longitude endereço do usuário (CENTROIDE)</t>
+    <t>customer_has_plus</t>
+  </si>
+  <si>
+    <t>se o usuários tinha serviço de assinatura ativo no momento da compra</t>
   </si>
   <si>
     <t>media_network</t>
@@ -631,67 +626,7 @@
     <t>De mídia veio a sessão Google Adwords, Facebook Ads, Twitter</t>
   </si>
   <si>
-    <t>External_user_id</t>
-  </si>
-  <si>
     <t>Data do primeiro pedido.</t>
-  </si>
-  <si>
-    <t>customer_latitude</t>
-  </si>
-  <si>
-    <t>latitude endereço do usuário (CENTROIDE)</t>
-  </si>
-  <si>
-    <t>media_attrib_date</t>
-  </si>
-  <si>
-    <t>Data da mídia</t>
-  </si>
-  <si>
-    <t>last_order_date</t>
-  </si>
-  <si>
-    <t>Data do último pedido.</t>
-  </si>
-  <si>
-    <t>customer_centroid_id</t>
-  </si>
-  <si>
-    <t>representação do centroide do usuário (concatenado do lat/long do usuário)</t>
-  </si>
-  <si>
-    <t>chs_fold</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>segmentação de centróides - urbanos de renda alta, média, baixa e não urbanos</t>
-  </si>
-  <si>
-    <t>days_to_reorder_at_datasource</t>
-  </si>
-  <si>
-    <t>Intervalo entre as compras at_datasource</t>
-  </si>
-  <si>
-    <t>customer_has_plus</t>
-  </si>
-  <si>
-    <t>se o usuários tinha serviço de assinatura ativo no momento da compra</t>
-  </si>
-  <si>
-    <t>chs_level</t>
-  </si>
-  <si>
-    <t>Nível do Fold : 1 a 5</t>
-  </si>
-  <si>
-    <t>days_to_reorder_at_concluded</t>
-  </si>
-  <si>
-    <t>Intervalo entre comprar considerando at_concluded</t>
   </si>
   <si>
     <t>customer_seg_status_last_month</t>
@@ -706,19 +641,22 @@
 Inactive - Não compou no mês anterior nem no retrasado, mas já foi comprador antes</t>
   </si>
   <si>
-    <t>latitude</t>
-  </si>
-  <si>
-    <t>Coordenada geográfica captada pelo endereço de entrega registrado, senão houver um endereço registrado, será captado a posição do dispositivo.</t>
-  </si>
-  <si>
-    <t>rfv_score</t>
-  </si>
-  <si>
-    <t>Score de recencia, frequência e valor.</t>
+    <t>media_attrib_date</t>
+  </si>
+  <si>
+    <t>Data da mídia</t>
+  </si>
+  <si>
+    <t>last_order_date</t>
+  </si>
+  <si>
+    <t>Data do último pedido.</t>
   </si>
   <si>
     <t>customer_seg_recency_bucket</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
   <si>
     <t>bucket referente a quão próximo foi feita a última compra:
@@ -729,13 +667,16 @@
 1 - Último pedido há mais de 91 dias</t>
   </si>
   <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>recency_days</t>
-  </si>
-  <si>
-    <t>Diferença em dias entre hoje e a última compra do usuário.</t>
+    <t>chs_fold</t>
+  </si>
+  <si>
+    <t>segmentação de centróides - urbanos de renda alta, média, baixa e não urbanos</t>
+  </si>
+  <si>
+    <t>days_to_reorder_at_datasource</t>
+  </si>
+  <si>
+    <t>Intervalo entre as compras at_datasource</t>
   </si>
   <si>
     <t>customer_seg_frequency_bucket</t>
@@ -749,42 +690,16 @@
 1 - Menos que 1 pedido/mês</t>
   </si>
   <si>
-    <t>event_start_at_amsp</t>
-  </si>
-  <si>
-    <t>Data e hora de inicío do evento</t>
-  </si>
-  <si>
-    <t>recency_days_bucket</t>
-  </si>
-  <si>
-    <t>Bucket de recency_days.</t>
-  </si>
-  <si>
-    <t>customer_seg_aov_bucket</t>
-  </si>
-  <si>
-    <t>bucket referente ao valor do ticket médio do usuário:
-5 - Acima de 70 reais
-4 - Acima de 49, até 70 reais
-3 - Acima de 35, até 49 reais
-2 - Acima de 21, até 35 reais
-1 - Até 21 reais</t>
-  </si>
-  <si>
-    <t>dt_amsp timestamp</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>baseada no fuso América/São Paulo</t>
-  </si>
-  <si>
-    <t>recency_days_bucket_description</t>
-  </si>
-  <si>
-    <t>Explica as quebras do recency_days_bucket.</t>
+    <t>chs_level</t>
+  </si>
+  <si>
+    <t>Nível do Fold : 1 a 5</t>
+  </si>
+  <si>
+    <t>days_to_reorder_at_concluded</t>
+  </si>
+  <si>
+    <t>Intervalo entre comprar considerando at_concluded</t>
   </si>
   <si>
     <t>customer_seg_merchant_offer_bucket</t>
@@ -798,16 +713,16 @@
 1 - Até 30 restaurantes</t>
   </si>
   <si>
-    <t>dt_partition</t>
-  </si>
-  <si>
-    <t>Coluna de particionamento</t>
-  </si>
-  <si>
-    <t>freq_last_91d</t>
-  </si>
-  <si>
-    <t>Frequência do usuário nos últimos 91 dias.</t>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>Coordenada geográfica captada pelo endereço de entrega registrado, senão houver um endereço registrado, será captado a posição do dispositivo.</t>
+  </si>
+  <si>
+    <t>rfv_score</t>
+  </si>
+  <si>
+    <t>Score de recencia, frequência e valor.</t>
   </si>
   <si>
     <t>customer_seg_benefits_sensitivity_bucket</t>
@@ -818,10 +733,13 @@
 Baixa - &lt; 33%</t>
   </si>
   <si>
-    <t>freq_last_91d_bucket</t>
-  </si>
-  <si>
-    <t>Bucket de frequência do usuário nos últimos 91 dias.</t>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>recency_days</t>
+  </si>
+  <si>
+    <t>Diferença em dias entre hoje e a última compra do usuário.</t>
   </si>
   <si>
     <t>customer_seg_marlin_tag</t>
@@ -834,10 +752,16 @@
 4 - Subsidy Carp</t>
   </si>
   <si>
-    <t>freq_last_91d_bucket_description</t>
-  </si>
-  <si>
-    <t>Explica as quebras do freq_last_91d_bucket.</t>
+    <t>event_start_at_amsp</t>
+  </si>
+  <si>
+    <t>Data e hora de inicío do evento</t>
+  </si>
+  <si>
+    <t>recency_days_bucket</t>
+  </si>
+  <si>
+    <t>Bucket de recency_days.</t>
   </si>
   <si>
     <t>customer_seg_gross_income_bucket</t>
@@ -852,16 +776,76 @@
 6 - Sem informação</t>
   </si>
   <si>
+    <t>dt_amsp timestamp</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>baseada no fuso América/São Paulo</t>
+  </si>
+  <si>
+    <t>recency_days_bucket_description</t>
+  </si>
+  <si>
+    <t>Explica as quebras do recency_days_bucket.</t>
+  </si>
+  <si>
+    <t>customer_seg_preffered_shift</t>
+  </si>
+  <si>
+    <t>segmentação do usuário de acordo com o shift com maior número de pedidos.</t>
+  </si>
+  <si>
+    <t>dt_partition</t>
+  </si>
+  <si>
+    <t>Coluna de particionamento</t>
+  </si>
+  <si>
+    <t>freq_last_91d</t>
+  </si>
+  <si>
+    <t>Frequência do usuário nos últimos 91 dias.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">short id do restaurante </t>
+  </si>
+  <si>
+    <t>freq_last_91d_bucket</t>
+  </si>
+  <si>
+    <t>Bucket de frequência do usuário nos últimos 91 dias.</t>
+  </si>
+  <si>
+    <t>merchant_city</t>
+  </si>
+  <si>
+    <t>cidade do restaurante</t>
+  </si>
+  <si>
+    <t>freq_last_91d_bucket_description</t>
+  </si>
+  <si>
+    <t>Explica as quebras do freq_last_91d_bucket.</t>
+  </si>
+  <si>
+    <t>merchant_district</t>
+  </si>
+  <si>
+    <t>bairro do restaurante</t>
+  </si>
+  <si>
     <t>avg_aov_last_91d</t>
   </si>
   <si>
     <t>Média de order_total dos últimos 91 dias.</t>
   </si>
   <si>
-    <t>customer_seg_preffered_shift</t>
-  </si>
-  <si>
-    <t>segmentação do usuário de acordo com o shift com maior número de pedidos.</t>
+    <t>merchant_centroid_id</t>
+  </si>
+  <si>
+    <t>centroid_id do merchant</t>
   </si>
   <si>
     <t>maturity_orders</t>
@@ -870,7 +854,10 @@
     <t>Total de pedidos realizados pelo usuário.</t>
   </si>
   <si>
-    <t xml:space="preserve">short id do restaurante </t>
+    <t>merchant_dish_type</t>
+  </si>
+  <si>
+    <t>tipo de cozinha do restaurante (Mercado é identificado com merchant_dish_type='Mercado')</t>
   </si>
   <si>
     <t>maturity_orders_bucket</t>
@@ -879,10 +866,10 @@
     <t>Bucket do total de pedidos realizados pelo usuário.</t>
   </si>
   <si>
-    <t>merchant_city</t>
-  </si>
-  <si>
-    <t>cidade do restaurante</t>
+    <t>distance_merchant_customer</t>
+  </si>
+  <si>
+    <t>distancia entre o endereço do usuário e o restaurante em metros</t>
   </si>
   <si>
     <t>maturity_orders_bucket_description</t>
@@ -891,10 +878,10 @@
     <t>Explica as quebras do maturity_orders_bucket_description .</t>
   </si>
   <si>
-    <t>merchant_district</t>
-  </si>
-  <si>
-    <t>bairro do restaurante</t>
+    <t>promo_is_promotion</t>
+  </si>
+  <si>
+    <t>pedido com promoção</t>
   </si>
   <si>
     <t>benefits_sensitivity</t>
@@ -903,10 +890,10 @@
     <t>Índice de sensibilidade a benefícios.</t>
   </si>
   <si>
-    <t>merchant_longitude</t>
-  </si>
-  <si>
-    <t>longitude do restaurante (CENTROIDE)</t>
+    <t>normal_items_quantity</t>
+  </si>
+  <si>
+    <t>quantidade dos itens não promocionados (promo_is_promotion = 0)</t>
   </si>
   <si>
     <t>benefits_sensitivity_bucket</t>
@@ -915,10 +902,10 @@
     <t>Bucket do índice de sensibilidade a beneficios.</t>
   </si>
   <si>
-    <t>merchant_latitude</t>
-  </si>
-  <si>
-    <t>latitude do restaurante (CENTROIDE)</t>
+    <t>promo_items_quantity</t>
+  </si>
+  <si>
+    <t>quantidade dos itens promocionados (promo_is_promotion = 1)</t>
   </si>
   <si>
     <t>preferred_shift_bucket</t>
@@ -927,10 +914,10 @@
     <t>Bucket de turno preferido.</t>
   </si>
   <si>
-    <t>merchant_centroid_id</t>
-  </si>
-  <si>
-    <t>centroid_id do merchant</t>
+    <t>order_lag_at_login</t>
+  </si>
+  <si>
+    <t>diferença entre o dia do pedido e o dia do pedido anterior</t>
   </si>
   <si>
     <t>preferred_shift_bucket_description</t>
@@ -939,10 +926,10 @@
     <t>Explica as quebras do preferred_shift_bucket.</t>
   </si>
   <si>
-    <t>merchant_dish_type</t>
-  </si>
-  <si>
-    <t>tipo de cozinha do restaurante (Mercado é identificado com merchant_dish_type='Mercado')</t>
+    <t>order_lead_at_login</t>
+  </si>
+  <si>
+    <t>diferença entre o dia do pedido e o dia do próximo pedido</t>
   </si>
   <si>
     <t>merchant_variety</t>
@@ -951,10 +938,10 @@
     <t>Índice de variedade de restaurantes nas compras do usuário.</t>
   </si>
   <si>
-    <t>distance_merchant_customer</t>
-  </si>
-  <si>
-    <t>distancia entre o endereço do usuário e o restaurante em metros</t>
+    <t>order_monthly_lead</t>
+  </si>
+  <si>
+    <t>diferença entre o mês do pedido e o mês do próximo pedido</t>
   </si>
   <si>
     <t>merchant_variety_bucket</t>
@@ -963,10 +950,10 @@
     <t>Bucket do índice de variedade de restaurantes nas compras do usuário.</t>
   </si>
   <si>
-    <t>promo_is_promotion</t>
-  </si>
-  <si>
-    <t>pedido com promoção</t>
+    <t>order_monthly_lag</t>
+  </si>
+  <si>
+    <t>diferença entre o mês do pedido e o mês do pedido anterior</t>
   </si>
   <si>
     <t>merchant_offer</t>
@@ -975,10 +962,7 @@
     <t>Cobertura de restaurantes no centroid_id do usuário.</t>
   </si>
   <si>
-    <t>normal_items_quantity</t>
-  </si>
-  <si>
-    <t>quantidade dos itens não promocionados (promo_is_promotion = 0)</t>
+    <t>data do pedido</t>
   </si>
   <si>
     <t>merchant_offer_bucket</t>
@@ -987,10 +971,10 @@
     <t>Bucket da cobertura de restaurantes no centroid_id do usuário.</t>
   </si>
   <si>
-    <t>promo_items_quantity</t>
-  </si>
-  <si>
-    <t>quantidade dos itens promocionados (promo_is_promotion = 1)</t>
+    <t>valid_order</t>
+  </si>
+  <si>
+    <t>pedido válido (isso é utilizado para identificar pedidos que não são teste de outros datasources ou informações mais antigas)</t>
   </si>
   <si>
     <t>merchant_offer_bucket_description</t>
@@ -999,10 +983,7 @@
     <t>Explica as quebras do merchant_offer_bucket .</t>
   </si>
   <si>
-    <t>order_lag_at_login</t>
-  </si>
-  <si>
-    <t>diferença entre o dia do pedido e o dia do pedido anterior</t>
+    <t>id da sessão do usuário (informação vinda direto do serviço de orders)</t>
   </si>
   <si>
     <t>top_dish_bucket</t>
@@ -1011,10 +992,10 @@
     <t>Bucket da cozinha favorita do usuário.</t>
   </si>
   <si>
-    <t>order_lead_at_login</t>
-  </si>
-  <si>
-    <t>diferença entre o dia do pedido e o dia do próximo pedido</t>
+    <t>Customer_id</t>
+  </si>
+  <si>
+    <t>id do usuário basedo no hash do email do usuário</t>
   </si>
   <si>
     <t>top_dish_bucket_description</t>
@@ -1023,38 +1004,29 @@
     <t>Explica as quebras do top_dish_bucket.</t>
   </si>
   <si>
-    <t>order_monthly_lead</t>
-  </si>
-  <si>
-    <t>diferença entre o mês do pedido e o mês do próximo pedido</t>
-  </si>
-  <si>
     <t>preferred_dishes</t>
   </si>
   <si>
     <t>Array contém as cozinhas favoritas do usuário.</t>
   </si>
   <si>
-    <t>order_monthly_lag</t>
-  </si>
-  <si>
-    <t>diferença entre o mês do pedido e o mês do pedido anterior</t>
-  </si>
-  <si>
     <t>preferred_dishes_code</t>
   </si>
   <si>
     <t>Array contém o código das cozinhas favoritas do usuário.</t>
   </si>
   <si>
-    <t>data do pedido</t>
+    <t>segmentation_month</t>
+  </si>
+  <si>
+    <t>mês da segmentação</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1062,17 +1034,27 @@
     </font>
     <font>
       <sz val="11.0"/>
-      <color rgb="FFD1D2D3"/>
+      <color rgb="FF434343"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
-      <color rgb="FFD1D2D3"/>
+      <color rgb="FF434343"/>
       <name val="Slack-Lato"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Slack-Lato"/>
     </font>
     <font>
       <b/>
@@ -1111,8 +1093,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF222529"/>
-        <bgColor rgb="FF222529"/>
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -1140,7 +1122,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border/>
     <border>
       <left style="thin">
@@ -1161,30 +1143,11 @@
         <color rgb="FF000000"/>
       </left>
     </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1197,61 +1160,55 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="3" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf borderId="0" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1472,10 +1429,9 @@
     <col customWidth="1" min="3" max="3" width="45.29"/>
     <col customWidth="1" min="5" max="5" width="34.29"/>
     <col customWidth="1" min="7" max="7" width="51.0"/>
-    <col customWidth="1" hidden="1" min="8" max="8" width="10.71"/>
-    <col customWidth="1" hidden="1" min="9" max="9" width="36.71"/>
-    <col hidden="1" min="10" max="10" width="14.43"/>
-    <col customWidth="1" hidden="1" min="11" max="11" width="52.57"/>
+    <col customWidth="1" min="8" max="8" width="10.71"/>
+    <col customWidth="1" min="9" max="9" width="36.71"/>
+    <col customWidth="1" min="11" max="11" width="52.57"/>
     <col customWidth="1" min="13" max="13" width="40.14"/>
     <col customWidth="1" min="15" max="15" width="43.71"/>
     <col customWidth="1" min="17" max="17" width="26.86"/>
@@ -1489,25 +1445,25 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
       <c r="H1" s="3"/>
       <c r="I1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
       <c r="L1" s="3"/>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="3"/>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="R1" s="4"/>
@@ -1521,53 +1477,53 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" ht="22.5" customHeight="1">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="3"/>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="3"/>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="P2" s="3"/>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="T2" s="3"/>
@@ -1579,53 +1535,53 @@
       <c r="Z2" s="3"/>
     </row>
     <row r="3" ht="22.5" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="9" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="3"/>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="11" t="s">
         <v>14</v>
       </c>
       <c r="L3" s="3"/>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="9" t="s">
         <v>15</v>
       </c>
       <c r="P3" s="3"/>
-      <c r="Q3" s="11" t="s">
+      <c r="Q3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="S3" s="11" t="s">
         <v>16</v>
       </c>
       <c r="T3" s="3"/>
@@ -1637,53 +1593,53 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4" ht="22.5" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="9" t="s">
         <v>20</v>
       </c>
       <c r="H4" s="3"/>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="9" t="s">
         <v>22</v>
       </c>
       <c r="L4" s="3"/>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="N4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="9" t="s">
         <v>24</v>
       </c>
       <c r="P4" s="3"/>
-      <c r="Q4" s="10" t="s">
+      <c r="Q4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="R4" s="12" t="s">
+      <c r="R4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="10" t="s">
+      <c r="S4" s="11" t="s">
         <v>26</v>
       </c>
       <c r="T4" s="3"/>
@@ -1695,53 +1651,53 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" ht="22.5" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="9" t="s">
         <v>30</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="14" t="s">
         <v>31</v>
       </c>
       <c r="L5" s="3"/>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="N5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="O5" s="9" t="s">
         <v>34</v>
       </c>
       <c r="P5" s="3"/>
-      <c r="Q5" s="10" t="s">
+      <c r="Q5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="R5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="S5" s="10" t="s">
+      <c r="S5" s="11" t="s">
         <v>36</v>
       </c>
       <c r="T5" s="3"/>
@@ -1753,53 +1709,53 @@
       <c r="Z5" s="3"/>
     </row>
     <row r="6" ht="22.5" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="9" t="s">
         <v>41</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="9" t="s">
         <v>43</v>
       </c>
       <c r="L6" s="3"/>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="O6" s="9" t="s">
         <v>45</v>
       </c>
       <c r="P6" s="3"/>
-      <c r="Q6" s="10" t="s">
+      <c r="Q6" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="R6" s="12" t="s">
+      <c r="R6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="S6" s="10" t="s">
+      <c r="S6" s="11" t="s">
         <v>47</v>
       </c>
       <c r="T6" s="3"/>
@@ -1811,53 +1767,53 @@
       <c r="Z6" s="3"/>
     </row>
     <row r="7" ht="22.5" customHeight="1">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="9" t="s">
         <v>51</v>
       </c>
       <c r="H7" s="3"/>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="9" t="s">
         <v>53</v>
       </c>
       <c r="L7" s="3"/>
-      <c r="M7" s="8" t="s">
+      <c r="M7" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="N7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="O7" s="9" t="s">
         <v>56</v>
       </c>
       <c r="P7" s="3"/>
-      <c r="Q7" s="10" t="s">
+      <c r="Q7" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="R7" s="12" t="s">
+      <c r="R7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="S7" s="10" t="s">
+      <c r="S7" s="11" t="s">
         <v>58</v>
       </c>
       <c r="T7" s="3"/>
@@ -1869,53 +1825,53 @@
       <c r="Z7" s="3"/>
     </row>
     <row r="8" ht="22.5" customHeight="1">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="J8" s="8" t="s">
+      <c r="K8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="N8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="O8" s="8" t="s">
+      <c r="O8" s="9" t="s">
         <v>66</v>
       </c>
       <c r="P8" s="3"/>
-      <c r="Q8" s="10" t="s">
+      <c r="Q8" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="R8" s="12" t="s">
+      <c r="R8" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="S8" s="10" t="s">
+      <c r="S8" s="11" t="s">
         <v>68</v>
       </c>
       <c r="T8" s="3"/>
@@ -1927,54 +1883,54 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" ht="22.5" customHeight="1">
-      <c r="A9" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="G9" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="N9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="J9" s="8" t="s">
+      <c r="O9" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="R9" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="K9" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="R9" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="S9" s="10" t="s">
-        <v>76</v>
+      <c r="S9" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
@@ -1985,48 +1941,54 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" ht="22.5" customHeight="1">
-      <c r="A10" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>78</v>
+      <c r="C10" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="9" t="s">
         <v>80</v>
       </c>
       <c r="H10" s="3"/>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="9" t="s">
         <v>82</v>
       </c>
       <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
+      <c r="M10" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="P10" s="3"/>
-      <c r="Q10" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="R10" s="12" t="s">
+      <c r="Q10" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="R10" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="S10" s="10" t="s">
-        <v>84</v>
+      <c r="S10" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
@@ -2037,48 +1999,48 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" ht="22.5" customHeight="1">
-      <c r="A11" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>86</v>
+      <c r="C11" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="E11" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>88</v>
+      <c r="G11" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="H11" s="3"/>
-      <c r="I11" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="J11" s="8" t="s">
+      <c r="I11" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="K11" s="8" t="s">
-        <v>90</v>
+      <c r="K11" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
-      <c r="Q11" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="R11" s="12" t="s">
+      <c r="Q11" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="R11" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="S11" s="10" t="s">
-        <v>92</v>
+      <c r="S11" s="11" t="s">
+        <v>95</v>
       </c>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
@@ -2089,48 +2051,48 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" ht="22.5" customHeight="1">
-      <c r="A12" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="8" t="s">
+      <c r="A12" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>94</v>
+      <c r="C12" s="9" t="s">
+        <v>97</v>
       </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F12" s="8" t="s">
+      <c r="E12" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="13" t="s">
-        <v>96</v>
+      <c r="G12" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="H12" s="3"/>
-      <c r="I12" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>98</v>
+      <c r="I12" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>101</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
-      <c r="Q12" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="R12" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="S12" s="10" t="s">
-        <v>101</v>
+      <c r="Q12" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="R12" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="S12" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
@@ -2141,48 +2103,48 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" ht="22.5" customHeight="1">
-      <c r="A13" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>103</v>
+      <c r="C13" s="9" t="s">
+        <v>106</v>
       </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F13" s="8" t="s">
+      <c r="E13" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="8" t="s">
-        <v>105</v>
+      <c r="G13" s="9" t="s">
+        <v>108</v>
       </c>
       <c r="H13" s="3"/>
-      <c r="I13" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>107</v>
+      <c r="I13" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
-      <c r="Q13" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="R13" s="12" t="s">
+      <c r="Q13" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="R13" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="S13" s="10" t="s">
-        <v>109</v>
+      <c r="S13" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
@@ -2193,48 +2155,48 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" ht="22.5" customHeight="1">
-      <c r="A14" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>111</v>
+      <c r="C14" s="9" t="s">
+        <v>115</v>
       </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="E14" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="8" t="s">
-        <v>113</v>
+      <c r="G14" s="9" t="s">
+        <v>117</v>
       </c>
       <c r="H14" s="3"/>
-      <c r="I14" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>116</v>
+      <c r="I14" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>119</v>
       </c>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
-      <c r="Q14" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="R14" s="12" t="s">
+      <c r="Q14" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="R14" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="S14" s="10" t="s">
-        <v>118</v>
+      <c r="S14" s="11" t="s">
+        <v>121</v>
       </c>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
@@ -2245,48 +2207,48 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" ht="22.5" customHeight="1">
-      <c r="A15" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>121</v>
+      <c r="A15" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>123</v>
       </c>
       <c r="D15" s="3"/>
-      <c r="E15" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="F15" s="8" t="s">
+      <c r="E15" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="8" t="s">
-        <v>123</v>
+      <c r="G15" s="9" t="s">
+        <v>125</v>
       </c>
       <c r="H15" s="3"/>
-      <c r="I15" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>125</v>
+      <c r="I15" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>127</v>
       </c>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
-      <c r="Q15" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="R15" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="S15" s="10" t="s">
-        <v>127</v>
+      <c r="Q15" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="R15" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="S15" s="11" t="s">
+        <v>129</v>
       </c>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
@@ -2297,48 +2259,48 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" ht="22.5" customHeight="1">
-      <c r="A16" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B16" s="8" t="s">
+      <c r="A16" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="J16" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>133</v>
+      <c r="K16" s="9" t="s">
+        <v>136</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
-      <c r="Q16" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="R16" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="S16" s="10" t="s">
-        <v>135</v>
+      <c r="Q16" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="R16" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="S16" s="11" t="s">
+        <v>138</v>
       </c>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
@@ -2349,48 +2311,48 @@
       <c r="Z16" s="3"/>
     </row>
     <row r="17" ht="22.5" customHeight="1">
-      <c r="A17" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="B17" s="8" t="s">
+      <c r="A17" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>137</v>
+      <c r="C17" s="9" t="s">
+        <v>140</v>
       </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>139</v>
+      <c r="E17" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>142</v>
       </c>
       <c r="H17" s="3"/>
-      <c r="I17" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="J17" s="8" t="s">
+      <c r="I17" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="J17" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K17" s="8" t="s">
-        <v>141</v>
+      <c r="K17" s="9" t="s">
+        <v>144</v>
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
-      <c r="Q17" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="R17" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="S17" s="10" t="s">
-        <v>143</v>
+      <c r="Q17" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="R17" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="S17" s="11" t="s">
+        <v>146</v>
       </c>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
@@ -2401,48 +2363,48 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" ht="22.5" customHeight="1">
-      <c r="A18" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B18" s="8" t="s">
+      <c r="A18" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>145</v>
+      <c r="C18" s="9" t="s">
+        <v>148</v>
       </c>
       <c r="D18" s="3"/>
-      <c r="E18" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>148</v>
+      <c r="E18" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>151</v>
       </c>
       <c r="H18" s="3"/>
-      <c r="I18" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="J18" s="8" t="s">
+      <c r="I18" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="J18" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K18" s="8" t="s">
-        <v>150</v>
+      <c r="K18" s="9" t="s">
+        <v>153</v>
       </c>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
-      <c r="Q18" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="R18" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="S18" s="10" t="s">
-        <v>152</v>
+      <c r="Q18" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="R18" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="S18" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
@@ -2453,48 +2415,48 @@
       <c r="Z18" s="3"/>
     </row>
     <row r="19" ht="22.5" customHeight="1">
-      <c r="A19" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>154</v>
+      <c r="A19" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>157</v>
       </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>156</v>
+      <c r="E19" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="H19" s="3"/>
-      <c r="I19" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="J19" s="8" t="s">
+      <c r="I19" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="J19" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K19" s="8" t="s">
-        <v>158</v>
+      <c r="K19" s="9" t="s">
+        <v>161</v>
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
-      <c r="Q19" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="R19" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="S19" s="10" t="s">
-        <v>160</v>
+      <c r="Q19" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="R19" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="S19" s="11" t="s">
+        <v>163</v>
       </c>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
@@ -2505,48 +2467,48 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" ht="22.5" customHeight="1">
-      <c r="A20" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>162</v>
+      <c r="A20" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="D20" s="3"/>
-      <c r="E20" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>164</v>
+      <c r="E20" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>167</v>
       </c>
       <c r="H20" s="3"/>
-      <c r="I20" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="J20" s="8" t="s">
+      <c r="I20" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="J20" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K20" s="8" t="s">
-        <v>166</v>
+      <c r="K20" s="9" t="s">
+        <v>169</v>
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
-      <c r="Q20" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="R20" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="S20" s="10" t="s">
-        <v>168</v>
+      <c r="Q20" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="R20" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="S20" s="11" t="s">
+        <v>171</v>
       </c>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
@@ -2557,48 +2519,48 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" ht="22.5" customHeight="1">
-      <c r="A21" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="B21" s="8" t="s">
+      <c r="A21" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="F21" s="8" t="s">
+      <c r="G21" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="J21" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>174</v>
+      <c r="K21" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
-      <c r="Q21" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="R21" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="S21" s="10" t="s">
-        <v>176</v>
+      <c r="Q21" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="R21" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="S21" s="11" t="s">
+        <v>179</v>
       </c>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
@@ -2609,48 +2571,48 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" ht="22.5" customHeight="1">
-      <c r="A22" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="B22" s="8" t="s">
+      <c r="A22" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>178</v>
+      <c r="C22" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="D22" s="3"/>
-      <c r="E22" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="F22" s="8" t="s">
+      <c r="E22" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="8" t="s">
-        <v>180</v>
+      <c r="G22" s="9" t="s">
+        <v>183</v>
       </c>
       <c r="H22" s="3"/>
-      <c r="I22" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="J22" s="8" t="s">
+      <c r="I22" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="J22" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K22" s="8" t="s">
-        <v>182</v>
+      <c r="K22" s="9" t="s">
+        <v>185</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
-      <c r="Q22" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="R22" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="S22" s="10" t="s">
-        <v>184</v>
+      <c r="Q22" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="R22" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="S22" s="11" t="s">
+        <v>187</v>
       </c>
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
@@ -2661,48 +2623,48 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" ht="22.5" customHeight="1">
-      <c r="A23" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="14" t="s">
+      <c r="A23" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>185</v>
+      <c r="C23" s="9" t="s">
+        <v>189</v>
       </c>
       <c r="D23" s="3"/>
-      <c r="E23" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="F23" s="8" t="s">
+      <c r="E23" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="F23" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="8" t="s">
-        <v>187</v>
+      <c r="G23" s="9" t="s">
+        <v>191</v>
       </c>
       <c r="H23" s="3"/>
-      <c r="I23" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>189</v>
+      <c r="I23" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>193</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
-      <c r="Q23" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="R23" s="12" t="s">
+      <c r="Q23" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="R23" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="S23" s="10" t="s">
-        <v>191</v>
+      <c r="S23" s="11" t="s">
+        <v>195</v>
       </c>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
@@ -2713,48 +2675,39 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" ht="22.5" customHeight="1">
-      <c r="A24" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="B24" s="15" t="s">
+      <c r="D24" s="3"/>
+      <c r="E24" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" s="8" t="s">
+      <c r="G24" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H24" s="3"/>
+      <c r="I24" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="J24" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G24" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K24" s="8" t="s">
-        <v>195</v>
+      <c r="K24" s="9" t="s">
+        <v>198</v>
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
-      <c r="Q24" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="R24" s="12" t="s">
+      <c r="Q24" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="R24" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="S24" s="10" t="s">
-        <v>197</v>
+      <c r="S24" s="11" t="s">
+        <v>200</v>
       </c>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
@@ -2769,38 +2722,38 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="F25" s="8" t="s">
+      <c r="E25" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="8" t="s">
-        <v>199</v>
+      <c r="G25" s="9" t="s">
+        <v>202</v>
       </c>
       <c r="H25" s="3"/>
-      <c r="I25" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>201</v>
+      <c r="I25" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>205</v>
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
-      <c r="Q25" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="R25" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="S25" s="10" t="s">
+      <c r="Q25" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="R25" s="13" t="s">
         <v>204</v>
+      </c>
+      <c r="S25" s="11" t="s">
+        <v>207</v>
       </c>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
@@ -2815,38 +2768,38 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="F26" s="8" t="s">
+      <c r="E26" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="8" t="s">
-        <v>206</v>
+      <c r="G26" s="9" t="s">
+        <v>209</v>
       </c>
       <c r="H26" s="3"/>
-      <c r="I26" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="J26" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="K26" s="8" t="s">
-        <v>208</v>
+      <c r="I26" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>211</v>
       </c>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
-      <c r="Q26" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="R26" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="S26" s="10" t="s">
-        <v>210</v>
+      <c r="Q26" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="R26" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="S26" s="11" t="s">
+        <v>213</v>
       </c>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
@@ -2861,38 +2814,38 @@
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="F27" s="8" t="s">
+      <c r="E27" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="F27" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="8" t="s">
-        <v>212</v>
+      <c r="G27" s="9" t="s">
+        <v>215</v>
       </c>
       <c r="H27" s="3"/>
-      <c r="I27" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>214</v>
+      <c r="I27" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>217</v>
       </c>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
-      <c r="Q27" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="R27" s="12" t="s">
+      <c r="Q27" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="R27" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="S27" s="10" t="s">
-        <v>216</v>
+      <c r="S27" s="11" t="s">
+        <v>219</v>
       </c>
       <c r="T27" s="3"/>
       <c r="U27" s="3"/>
@@ -2907,38 +2860,38 @@
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="F28" s="8" t="s">
+      <c r="E28" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="F28" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G28" s="8" t="s">
-        <v>218</v>
+      <c r="G28" s="9" t="s">
+        <v>221</v>
       </c>
       <c r="H28" s="3"/>
-      <c r="I28" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="K28" s="8" t="s">
-        <v>220</v>
+      <c r="I28" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>223</v>
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
-      <c r="Q28" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="R28" s="12" t="s">
+      <c r="Q28" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="R28" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="S28" s="10" t="s">
-        <v>216</v>
+      <c r="S28" s="11" t="s">
+        <v>219</v>
       </c>
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
@@ -2953,38 +2906,38 @@
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>223</v>
+      <c r="E29" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>226</v>
       </c>
       <c r="H29" s="3"/>
-      <c r="I29" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="J29" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="K29" s="8" t="s">
-        <v>225</v>
+      <c r="I29" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>228</v>
       </c>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
-      <c r="Q29" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="R29" s="12" t="s">
+      <c r="Q29" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="R29" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="S29" s="10" t="s">
-        <v>227</v>
+      <c r="S29" s="11" t="s">
+        <v>230</v>
       </c>
       <c r="T29" s="3"/>
       <c r="U29" s="3"/>
@@ -2999,38 +2952,38 @@
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>229</v>
+      <c r="E30" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>232</v>
       </c>
       <c r="H30" s="3"/>
-      <c r="I30" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="K30" s="8" t="s">
-        <v>231</v>
+      <c r="I30" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>234</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
-      <c r="Q30" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="R30" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="S30" s="10" t="s">
-        <v>234</v>
+      <c r="Q30" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="R30" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="S30" s="11" t="s">
+        <v>237</v>
       </c>
       <c r="T30" s="3"/>
       <c r="U30" s="3"/>
@@ -3045,38 +2998,38 @@
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="F31" s="8" t="s">
+      <c r="E31" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="F31" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G31" s="8" t="s">
-        <v>236</v>
+      <c r="G31" s="9" t="s">
+        <v>239</v>
       </c>
       <c r="H31" s="3"/>
-      <c r="I31" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="K31" s="8" t="s">
-        <v>238</v>
+      <c r="I31" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K31" s="9" t="s">
+        <v>241</v>
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
-      <c r="Q31" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="R31" s="12" t="s">
+      <c r="Q31" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="R31" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="S31" s="10" t="s">
-        <v>240</v>
+      <c r="S31" s="11" t="s">
+        <v>243</v>
       </c>
       <c r="T31" s="3"/>
       <c r="U31" s="3"/>
@@ -3091,24 +3044,24 @@
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
-      <c r="E32" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="F32" s="8" t="s">
+      <c r="E32" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="F32" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G32" s="8" t="s">
-        <v>242</v>
+      <c r="G32" s="9" t="s">
+        <v>245</v>
       </c>
       <c r="H32" s="3"/>
-      <c r="I32" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="J32" s="8" t="s">
+      <c r="I32" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J32" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K32" s="16" t="s">
-        <v>244</v>
+      <c r="K32" s="9" t="s">
+        <v>246</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -3128,24 +3081,24 @@
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>246</v>
+      <c r="E33" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>248</v>
       </c>
       <c r="H33" s="3"/>
-      <c r="I33" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="J33" s="8" t="s">
+      <c r="I33" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="J33" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K33" s="8" t="s">
-        <v>248</v>
+      <c r="K33" s="9" t="s">
+        <v>250</v>
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -3165,24 +3118,24 @@
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
-      <c r="E34" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="F34" s="8" t="s">
+      <c r="E34" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="F34" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="8" t="s">
-        <v>250</v>
+      <c r="G34" s="9" t="s">
+        <v>252</v>
       </c>
       <c r="H34" s="3"/>
-      <c r="I34" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="J34" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="K34" s="8" t="s">
-        <v>252</v>
+      <c r="I34" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>254</v>
       </c>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
@@ -3202,24 +3155,24 @@
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="F35" s="8" t="s">
+      <c r="E35" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="F35" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G35" s="8" t="s">
-        <v>254</v>
+      <c r="G35" s="9" t="s">
+        <v>256</v>
       </c>
       <c r="H35" s="3"/>
-      <c r="I35" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="J35" s="8" t="s">
+      <c r="I35" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="J35" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K35" s="8" t="s">
-        <v>256</v>
+      <c r="K35" s="9" t="s">
+        <v>258</v>
       </c>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
@@ -3239,33 +3192,33 @@
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="F36" s="8" t="s">
+      <c r="E36" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="F36" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G36" s="8" t="s">
-        <v>258</v>
+      <c r="G36" s="9" t="s">
+        <v>260</v>
       </c>
       <c r="H36" s="3"/>
-      <c r="I36" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="J36" s="8" t="s">
+      <c r="I36" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="J36" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K36" s="8" t="s">
-        <v>259</v>
+      <c r="K36" s="9" t="s">
+        <v>262</v>
       </c>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
-      <c r="Q36" s="17"/>
-      <c r="R36" s="18"/>
-      <c r="S36" s="17"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="17"/>
+      <c r="S36" s="16"/>
       <c r="T36" s="3"/>
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
@@ -3279,33 +3232,33 @@
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>261</v>
+      <c r="E37" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>264</v>
       </c>
       <c r="H37" s="3"/>
-      <c r="I37" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K37" s="8" t="s">
-        <v>263</v>
+      <c r="I37" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K37" s="9" t="s">
+        <v>266</v>
       </c>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
-      <c r="Q37" s="19"/>
-      <c r="R37" s="20"/>
-      <c r="S37" s="19"/>
+      <c r="Q37" s="18"/>
+      <c r="R37" s="19"/>
+      <c r="S37" s="18"/>
       <c r="T37" s="3"/>
       <c r="U37" s="3"/>
       <c r="V37" s="3"/>
@@ -3319,33 +3272,33 @@
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="F38" s="8" t="s">
+      <c r="E38" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="F38" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G38" s="8" t="s">
-        <v>265</v>
+      <c r="G38" s="9" t="s">
+        <v>268</v>
       </c>
       <c r="H38" s="3"/>
-      <c r="I38" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="J38" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K38" s="8" t="s">
-        <v>267</v>
+      <c r="I38" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K38" s="9" t="s">
+        <v>270</v>
       </c>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
-      <c r="Q38" s="17"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="17"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="17"/>
+      <c r="S38" s="16"/>
       <c r="T38" s="3"/>
       <c r="U38" s="3"/>
       <c r="V38" s="3"/>
@@ -3359,33 +3312,33 @@
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
-      <c r="E39" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="F39" s="8" t="s">
+      <c r="E39" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="F39" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G39" s="8" t="s">
-        <v>269</v>
+      <c r="G39" s="9" t="s">
+        <v>272</v>
       </c>
       <c r="H39" s="3"/>
-      <c r="I39" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="J39" s="8" t="s">
+      <c r="I39" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="J39" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="K39" s="8" t="s">
-        <v>271</v>
+      <c r="K39" s="9" t="s">
+        <v>274</v>
       </c>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
-      <c r="Q39" s="19"/>
-      <c r="R39" s="20"/>
-      <c r="S39" s="19"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="19"/>
+      <c r="S39" s="18"/>
       <c r="T39" s="3"/>
       <c r="U39" s="3"/>
       <c r="V39" s="3"/>
@@ -3399,33 +3352,33 @@
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
-      <c r="E40" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="F40" s="8" t="s">
+      <c r="E40" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="F40" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G40" s="8" t="s">
-        <v>273</v>
+      <c r="G40" s="9" t="s">
+        <v>276</v>
       </c>
       <c r="H40" s="3"/>
-      <c r="I40" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="J40" s="8" t="s">
+      <c r="I40" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="J40" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="K40" s="8" t="s">
-        <v>275</v>
+      <c r="K40" s="9" t="s">
+        <v>278</v>
       </c>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
-      <c r="Q40" s="17"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="17"/>
+      <c r="Q40" s="16"/>
+      <c r="R40" s="17"/>
+      <c r="S40" s="16"/>
       <c r="T40" s="3"/>
       <c r="U40" s="3"/>
       <c r="V40" s="3"/>
@@ -3439,33 +3392,33 @@
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
-      <c r="E41" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>277</v>
+      <c r="E41" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>280</v>
       </c>
       <c r="H41" s="3"/>
-      <c r="I41" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="J41" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K41" s="8" t="s">
-        <v>279</v>
+      <c r="I41" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="J41" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="K41" s="9" t="s">
+        <v>282</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
-      <c r="Q41" s="19"/>
-      <c r="R41" s="20"/>
-      <c r="S41" s="19"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="19"/>
+      <c r="S41" s="18"/>
       <c r="T41" s="3"/>
       <c r="U41" s="3"/>
       <c r="V41" s="3"/>
@@ -3479,33 +3432,33 @@
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
-      <c r="E42" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="F42" s="8" t="s">
+      <c r="E42" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="F42" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="8" t="s">
-        <v>281</v>
+      <c r="G42" s="9" t="s">
+        <v>284</v>
       </c>
       <c r="H42" s="3"/>
-      <c r="I42" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="J42" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K42" s="8" t="s">
-        <v>283</v>
+      <c r="I42" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="J42" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="K42" s="9" t="s">
+        <v>286</v>
       </c>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
-      <c r="Q42" s="17"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="17"/>
+      <c r="Q42" s="16"/>
+      <c r="R42" s="17"/>
+      <c r="S42" s="16"/>
       <c r="T42" s="3"/>
       <c r="U42" s="3"/>
       <c r="V42" s="3"/>
@@ -3519,33 +3472,33 @@
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
-      <c r="E43" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="F43" s="8" t="s">
+      <c r="E43" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="F43" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G43" s="8" t="s">
-        <v>285</v>
+      <c r="G43" s="9" t="s">
+        <v>288</v>
       </c>
       <c r="H43" s="3"/>
-      <c r="I43" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="J43" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="K43" s="8" t="s">
-        <v>287</v>
+      <c r="I43" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="J43" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="K43" s="9" t="s">
+        <v>290</v>
       </c>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
-      <c r="Q43" s="19"/>
-      <c r="R43" s="20"/>
-      <c r="S43" s="21"/>
+      <c r="Q43" s="18"/>
+      <c r="R43" s="19"/>
+      <c r="S43" s="20"/>
       <c r="T43" s="3"/>
       <c r="U43" s="3"/>
       <c r="V43" s="3"/>
@@ -3559,33 +3512,33 @@
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
-      <c r="E44" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="F44" s="8" t="s">
+      <c r="E44" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="F44" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G44" s="8" t="s">
-        <v>289</v>
+      <c r="G44" s="9" t="s">
+        <v>292</v>
       </c>
       <c r="H44" s="3"/>
-      <c r="I44" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="J44" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="K44" s="8" t="s">
-        <v>291</v>
+      <c r="I44" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="J44" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="K44" s="9" t="s">
+        <v>294</v>
       </c>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
-      <c r="Q44" s="17"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="17"/>
+      <c r="Q44" s="16"/>
+      <c r="R44" s="17"/>
+      <c r="S44" s="16"/>
       <c r="T44" s="3"/>
       <c r="U44" s="3"/>
       <c r="V44" s="3"/>
@@ -3599,24 +3552,24 @@
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
-      <c r="E45" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="F45" s="8" t="s">
+      <c r="E45" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="F45" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G45" s="8" t="s">
-        <v>293</v>
+      <c r="G45" s="9" t="s">
+        <v>296</v>
       </c>
       <c r="H45" s="3"/>
-      <c r="I45" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="J45" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="K45" s="8" t="s">
-        <v>295</v>
+      <c r="I45" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J45" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K45" s="9" t="s">
+        <v>297</v>
       </c>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
@@ -3636,24 +3589,24 @@
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
-      <c r="E46" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="G46" s="8" t="s">
-        <v>297</v>
+      <c r="E46" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>299</v>
       </c>
       <c r="H46" s="3"/>
-      <c r="I46" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="J46" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="K46" s="8" t="s">
-        <v>299</v>
+      <c r="I46" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="J46" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K46" s="9" t="s">
+        <v>301</v>
       </c>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
@@ -3673,24 +3626,24 @@
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
-      <c r="E47" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="F47" s="8" t="s">
+      <c r="E47" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="F47" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G47" s="8" t="s">
-        <v>301</v>
+      <c r="G47" s="9" t="s">
+        <v>303</v>
       </c>
       <c r="H47" s="3"/>
-      <c r="I47" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="J47" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="K47" s="8" t="s">
-        <v>303</v>
+      <c r="I47" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J47" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K47" s="9" t="s">
+        <v>304</v>
       </c>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
@@ -3710,24 +3663,24 @@
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
-      <c r="E48" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="G48" s="8" t="s">
+      <c r="E48" s="9" t="s">
         <v>305</v>
       </c>
+      <c r="F48" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>306</v>
+      </c>
       <c r="H48" s="3"/>
-      <c r="I48" s="8" t="s">
-        <v>306</v>
-      </c>
-      <c r="J48" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="K48" s="8" t="s">
+      <c r="I48" s="9" t="s">
         <v>307</v>
+      </c>
+      <c r="J48" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K48" s="9" t="s">
+        <v>308</v>
       </c>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
@@ -3747,25 +3700,16 @@
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
-      <c r="E49" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="F49" s="8" t="s">
+      <c r="E49" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="F49" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G49" s="8" t="s">
-        <v>309</v>
+      <c r="G49" s="9" t="s">
+        <v>310</v>
       </c>
       <c r="H49" s="3"/>
-      <c r="I49" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="J49" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="K49" s="8" t="s">
-        <v>311</v>
-      </c>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
@@ -3784,25 +3728,16 @@
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
-      <c r="E50" s="8" t="s">
+      <c r="E50" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G50" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="F50" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="G50" s="8" t="s">
-        <v>313</v>
-      </c>
       <c r="H50" s="3"/>
-      <c r="I50" s="8" t="s">
-        <v>314</v>
-      </c>
-      <c r="J50" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="K50" s="8" t="s">
-        <v>315</v>
-      </c>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
@@ -3821,25 +3756,16 @@
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
-      <c r="E51" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="G51" s="8" t="s">
-        <v>317</v>
+      <c r="E51" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>314</v>
       </c>
       <c r="H51" s="3"/>
-      <c r="I51" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="J51" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K51" s="8" t="s">
-        <v>318</v>
-      </c>
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
@@ -3858,9 +3784,15 @@
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
+      <c r="E52" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>316</v>
+      </c>
       <c r="H52" s="3"/>
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>

</xml_diff>